<commit_message>
pushing saved trash dataset (excel file)
</commit_message>
<xml_diff>
--- a/hw2 data/trash_wheel_data.xlsx
+++ b/hw2 data/trash_wheel_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aelga\OneDrive\Documents\Class Work\Data Science\Homeworks\p8105_hw2_are2132\hw2 data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20977614-19F4-4CFE-ADBF-8B23673E81AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B94CEB-5B6C-4846-B933-B8C23B067374}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="18220" windowHeight="11620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18220" windowHeight="11620" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mr. Trash Wheel" sheetId="3" r:id="rId1"/>
@@ -1747,10 +1747,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O338"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" outlineLevelRow="2"/>
@@ -17206,7 +17206,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O203"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -21390,7 +21390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>